<commit_message>
all highlighting works!  But also shows empty
</commit_message>
<xml_diff>
--- a/dashboard/assets/data/test.xlsx
+++ b/dashboard/assets/data/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mo/Desktop/data-runners/dashboard/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D316DFF2-CB75-2E4F-9E86-E917B37A92A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840FB51F-EE01-DE47-868A-A1731D49543B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15980" xr2:uid="{517C14D0-415C-6C45-9CD3-0757733CD81B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="132">
   <si>
     <t>GPA</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>chocolate, chips, ice cream</t>
-  </si>
-  <si>
-    <t>frozen yogurt, pizza, fast food</t>
   </si>
   <si>
     <t>Pizza, Mac and cheese, ice cream</t>
@@ -789,7 +786,7 @@
   <dimension ref="A1:D126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -802,10 +799,10 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" t="s">
         <v>127</v>
-      </c>
-      <c r="D1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -819,7 +816,7 @@
         <v>187</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -837,11 +834,11 @@
       <c r="A4">
         <v>3.3</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
+      <c r="B4">
+        <v>5555</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -849,10 +846,10 @@
         <v>3.2</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -860,7 +857,7 @@
         <v>3.5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>190</v>
@@ -874,7 +871,7 @@
         <v>2.25</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>190</v>
@@ -899,7 +896,7 @@
         <v>3.3</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>137</v>
@@ -910,7 +907,7 @@
         <v>3.3</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>180</v>
@@ -932,7 +929,7 @@
         <v>3.5</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>116</v>
@@ -943,7 +940,7 @@
         <v>3.9039999999999999</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>110</v>
@@ -954,7 +951,7 @@
         <v>3.4</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>264</v>
@@ -965,7 +962,7 @@
         <v>3.6</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>123</v>
@@ -987,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>180</v>
@@ -998,7 +995,7 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>145</v>
@@ -1009,7 +1006,7 @@
         <v>3.6</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>170</v>
@@ -1020,7 +1017,7 @@
         <v>3.4</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>135</v>
@@ -1031,7 +1028,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>165</v>
@@ -1042,7 +1039,7 @@
         <v>3.3</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>175</v>
@@ -1053,7 +1050,7 @@
         <v>3.87</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23">
         <v>195</v>
@@ -1064,7 +1061,7 @@
         <v>3.7</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24">
         <v>185</v>
@@ -1075,7 +1072,7 @@
         <v>3.7</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <v>185</v>
@@ -1086,7 +1083,7 @@
         <v>3.9</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <v>105</v>
@@ -1097,7 +1094,7 @@
         <v>2.8</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27">
         <v>125</v>
@@ -1108,7 +1105,7 @@
         <v>3.7</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28">
         <v>160</v>
@@ -1119,7 +1116,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29">
         <v>175</v>
@@ -1130,7 +1127,7 @@
         <v>3.2</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30">
         <v>180</v>
@@ -1141,7 +1138,7 @@
         <v>3.5</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>167</v>
@@ -1152,7 +1149,7 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>115</v>
@@ -1163,7 +1160,7 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33">
         <v>205</v>
@@ -1174,7 +1171,7 @@
         <v>3.4</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -1185,7 +1182,7 @@
         <v>2.8</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35">
         <v>128</v>
@@ -1196,7 +1193,7 @@
         <v>3.65</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C36">
         <v>150</v>
@@ -1207,7 +1204,7 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37">
         <v>150</v>
@@ -1218,7 +1215,7 @@
         <v>3.7</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38">
         <v>150</v>
@@ -1229,7 +1226,7 @@
         <v>3.4</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39">
         <v>170</v>
@@ -1240,7 +1237,7 @@
         <v>3.89</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40">
         <v>150</v>
@@ -1251,7 +1248,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41">
         <v>175</v>
@@ -1262,7 +1259,7 @@
         <v>3.4</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42">
         <v>140</v>
@@ -1273,7 +1270,7 @@
         <v>2.9</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43">
         <v>120</v>
@@ -1284,7 +1281,7 @@
         <v>3.6</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C44">
         <v>135</v>
@@ -1295,7 +1292,7 @@
         <v>3.5</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45">
         <v>100</v>
@@ -1306,7 +1303,7 @@
         <v>3.2</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46">
         <v>170</v>
@@ -1317,7 +1314,7 @@
         <v>3.605</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C47">
         <v>113</v>
@@ -1328,7 +1325,7 @@
         <v>3.8</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C48">
         <v>168</v>
@@ -1339,7 +1336,7 @@
         <v>2.8</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C49">
         <v>145</v>
@@ -1350,7 +1347,7 @@
         <v>3.5</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C50">
         <v>155</v>
@@ -1361,7 +1358,7 @@
         <v>3.83</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C51">
         <v>150</v>
@@ -1372,7 +1369,7 @@
         <v>3.6</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C52">
         <v>169</v>
@@ -1383,7 +1380,7 @@
         <v>3.3</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C53">
         <v>185</v>
@@ -1394,7 +1391,7 @@
         <v>3.3</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54">
         <v>200</v>
@@ -1405,7 +1402,7 @@
         <v>3.2919999999999998</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C55">
         <v>265</v>
@@ -1416,7 +1413,7 @@
         <v>3.5</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C56">
         <v>165</v>
@@ -1427,7 +1424,7 @@
         <v>3.35</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C57">
         <v>192</v>
@@ -1438,7 +1435,7 @@
         <v>3.8</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C58">
         <v>175</v>
@@ -1449,7 +1446,7 @@
         <v>2.8</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C59">
         <v>140</v>
@@ -1460,7 +1457,7 @@
         <v>3.5</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C60">
         <v>155</v>
@@ -1471,7 +1468,7 @@
         <v>3.7</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C61">
         <v>155</v>
@@ -1482,7 +1479,7 @@
         <v>3.6</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C62">
         <v>135</v>
@@ -1493,7 +1490,7 @@
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C63">
         <v>118</v>
@@ -1504,7 +1501,7 @@
         <v>3.9</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C64">
         <v>210</v>
@@ -1515,7 +1512,7 @@
         <v>2.6</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C65">
         <v>180</v>
@@ -1526,7 +1523,7 @@
         <v>3.5</v>
       </c>
       <c r="B66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C66">
         <v>140</v>
@@ -1537,7 +1534,7 @@
         <v>3.2</v>
       </c>
       <c r="B67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C67">
         <v>112</v>
@@ -1548,7 +1545,7 @@
         <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C68">
         <v>125</v>
@@ -1559,10 +1556,10 @@
         <v>3.6</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C69" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1570,7 +1567,7 @@
         <v>3.2</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C70">
         <v>145</v>
@@ -1581,7 +1578,7 @@
         <v>3.67</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C71">
         <v>130</v>
@@ -1592,7 +1589,7 @@
         <v>3.73</v>
       </c>
       <c r="B72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C72">
         <v>140</v>
@@ -1603,7 +1600,7 @@
         <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C73">
         <v>140</v>
@@ -1614,7 +1611,7 @@
         <v>3.1</v>
       </c>
       <c r="B74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C74">
         <v>140</v>
@@ -1625,7 +1622,7 @@
         <v>3</v>
       </c>
       <c r="B75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C75">
         <v>200</v>
@@ -1647,7 +1644,7 @@
         <v>3</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C77">
         <v>120</v>
@@ -1658,7 +1655,7 @@
         <v>3.7</v>
       </c>
       <c r="B78" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C78">
         <v>150</v>
@@ -1669,7 +1666,7 @@
         <v>3.1</v>
       </c>
       <c r="B79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C79">
         <v>200</v>
@@ -1680,7 +1677,7 @@
         <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C80">
         <v>135</v>
@@ -1691,7 +1688,7 @@
         <v>3.9</v>
       </c>
       <c r="B81" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C81">
         <v>145</v>
@@ -1702,7 +1699,7 @@
         <v>3.4</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C82">
         <v>130</v>
@@ -1713,7 +1710,7 @@
         <v>3.5</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C83">
         <v>190</v>
@@ -1724,7 +1721,7 @@
         <v>3.7</v>
       </c>
       <c r="B84" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C84">
         <v>170</v>
@@ -1735,7 +1732,7 @@
         <v>3.7</v>
       </c>
       <c r="B85" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C85">
         <v>127</v>
@@ -1746,7 +1743,7 @@
         <v>3.83</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C86">
         <v>167</v>
@@ -1757,7 +1754,7 @@
         <v>2.6</v>
       </c>
       <c r="B87" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C87">
         <v>140</v>
@@ -1768,7 +1765,7 @@
         <v>3</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C88">
         <v>190</v>
@@ -1779,7 +1776,7 @@
         <v>3.2</v>
       </c>
       <c r="B89" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C89">
         <v>155</v>
@@ -1790,7 +1787,7 @@
         <v>3.5</v>
       </c>
       <c r="B90" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C90">
         <v>175</v>
@@ -1801,7 +1798,7 @@
         <v>3.2</v>
       </c>
       <c r="B91" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C91">
         <v>129</v>
@@ -1812,7 +1809,7 @@
         <v>3.68</v>
       </c>
       <c r="B92" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C92">
         <v>260</v>
@@ -1823,7 +1820,7 @@
         <v>3.8</v>
       </c>
       <c r="B93" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C93">
         <v>135</v>
@@ -1834,7 +1831,7 @@
         <v>3.3</v>
       </c>
       <c r="B94" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C94">
         <v>190</v>
@@ -1845,7 +1842,7 @@
         <v>3.2</v>
       </c>
       <c r="B95" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C95">
         <v>165</v>
@@ -1856,7 +1853,7 @@
         <v>3.75</v>
       </c>
       <c r="B96" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C96">
         <v>175</v>
@@ -1867,7 +1864,7 @@
         <v>3.5</v>
       </c>
       <c r="B97" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C97">
         <v>184</v>
@@ -1878,7 +1875,7 @@
         <v>3.92</v>
       </c>
       <c r="B98" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C98">
         <v>210</v>
@@ -1889,7 +1886,7 @@
         <v>3.9</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C99">
         <v>155</v>
@@ -1900,7 +1897,7 @@
         <v>3.9</v>
       </c>
       <c r="B100" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C100">
         <v>185</v>
@@ -1911,7 +1908,7 @@
         <v>3.2</v>
       </c>
       <c r="B101" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C101">
         <v>165</v>
@@ -1922,7 +1919,7 @@
         <v>3.5</v>
       </c>
       <c r="B102" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C102">
         <v>125</v>
@@ -1933,7 +1930,7 @@
         <v>3.4</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C103">
         <v>160</v>
@@ -1944,7 +1941,7 @@
         <v>1</v>
       </c>
       <c r="B104" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C104">
         <v>135</v>
@@ -1955,7 +1952,7 @@
         <v>3.7</v>
       </c>
       <c r="B105" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C105">
         <v>130</v>
@@ -1966,7 +1963,7 @@
         <v>4</v>
       </c>
       <c r="B106" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C106">
         <v>230</v>
@@ -1977,7 +1974,7 @@
         <v>3</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C107">
         <v>125</v>
@@ -1988,7 +1985,7 @@
         <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C108">
         <v>130</v>
@@ -1999,7 +1996,7 @@
         <v>3.8</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C109">
         <v>165</v>
@@ -2010,7 +2007,7 @@
         <v>3.8</v>
       </c>
       <c r="B110" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C110">
         <v>128</v>
@@ -2021,7 +2018,7 @@
         <v>3.4</v>
       </c>
       <c r="B111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C111">
         <v>200</v>
@@ -2032,7 +2029,7 @@
         <v>3.7</v>
       </c>
       <c r="B112" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C112">
         <v>160</v>
@@ -2043,7 +2040,7 @@
         <v>2.9</v>
       </c>
       <c r="B113" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C113">
         <v>170</v>
@@ -2054,7 +2051,7 @@
         <v>3.9</v>
       </c>
       <c r="B114" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C114">
         <v>129</v>
@@ -2065,7 +2062,7 @@
         <v>3.6</v>
       </c>
       <c r="B115" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C115">
         <v>170</v>
@@ -2076,7 +2073,7 @@
         <v>2.8</v>
       </c>
       <c r="B116" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C116">
         <v>138</v>
@@ -2087,7 +2084,7 @@
         <v>3.3</v>
       </c>
       <c r="B117" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C117">
         <v>150</v>
@@ -2098,7 +2095,7 @@
         <v>3.4</v>
       </c>
       <c r="B118" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C118">
         <v>170</v>
@@ -2109,7 +2106,7 @@
         <v>3.77</v>
       </c>
       <c r="B119" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C119">
         <v>113</v>
@@ -2120,7 +2117,7 @@
         <v>3.63</v>
       </c>
       <c r="B120" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C120">
         <v>140</v>
@@ -2131,7 +2128,7 @@
         <v>3.2</v>
       </c>
       <c r="B121" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C121">
         <v>185</v>
@@ -2142,7 +2139,7 @@
         <v>3.5</v>
       </c>
       <c r="B122" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C122">
         <v>156</v>
@@ -2153,7 +2150,7 @@
         <v>3</v>
       </c>
       <c r="B123" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C123">
         <v>180</v>
@@ -2164,7 +2161,7 @@
         <v>3.8820000000000001</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C124">
         <v>120</v>
@@ -2175,7 +2172,7 @@
         <v>3</v>
       </c>
       <c r="B125" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C125">
         <v>135</v>
@@ -2186,7 +2183,7 @@
         <v>3.9</v>
       </c>
       <c r="B126" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C126">
         <v>135</v>

</xml_diff>